<commit_message>
thêm use case list
</commit_message>
<xml_diff>
--- a/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirementand Business Rule.xlsx
+++ b/Requirement Management/Software Requirement Specification/[HRM]Funtional Requirementand Business Rule.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Funtional Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Business Rule" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Use case" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funtional Requirements'!$A$4:$C$4</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>Description</t>
   </si>
@@ -244,6 +245,18 @@
   </si>
   <si>
     <t>Information in excel file must be placed in appropriate order</t>
+  </si>
+  <si>
+    <t>HRM Use Case</t>
+  </si>
+  <si>
+    <t>HRM.FE7.FR1.UC1</t>
+  </si>
+  <si>
+    <t>HRM.FE7.FR1.UC2</t>
+  </si>
+  <si>
+    <t>Actions/ Brief Description</t>
   </si>
 </sst>
 </file>
@@ -337,9 +350,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -347,6 +357,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,36 +670,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="121.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="11.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -706,328 +719,328 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>17</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>18</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>19</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>20</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>21</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>22</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>23</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>24</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:C4"/>
@@ -1043,38 +1056,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="11.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1091,208 +1104,208 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>17</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>18</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>19</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>20</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>21</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>22</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>23</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>24</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1304,6 +1317,259 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>23</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1312,64 +1578,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="37.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="37.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1377,57 +1643,57 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>